<commit_message>
* Added relative information to summary report. * Changed NaN text to <NaN>.
</commit_message>
<xml_diff>
--- a/tests/data/desired/summaryreport.xlsx
+++ b/tests/data/desired/summaryreport.xlsx
@@ -15,13 +15,13 @@
     <sheet name="rcomp" r:id="rId9" sheetId="7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">full!$A$1:$B$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">left!$A$1:$B$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="true">right!$A$1:$B$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="true">inner!$A$1:$B$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="true">complement!$A$1:$B$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="true">lcomp!$A$1:$B$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="true">rcomp!$A$1:$B$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">full!$A$1:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">left!$A$1:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="true">right!$A$1:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="true">inner!$A$1:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="true">complement!$A$1:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="true">lcomp!$A$1:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="true">rcomp!$A$1:$C$9</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -102,10 +102,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -120,6 +121,7 @@
   <cols>
     <col min="1" max="1" width="35.66015625" customWidth="true"/>
     <col min="2" max="2" width="10.32421875" customWidth="true"/>
+    <col min="3" max="3" width="12.4609375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -133,6 +135,11 @@
           <t>Value</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Relative</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -143,6 +150,9 @@
       <c r="B2" t="n">
         <v>140.0</v>
       </c>
+      <c r="C2" s="3" t="n">
+        <v>0.14014014014014015</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -153,6 +163,9 @@
       <c r="B3" t="n">
         <v>960.0</v>
       </c>
+      <c r="C3" s="3" t="n">
+        <v>0.960960960960961</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -163,6 +176,9 @@
       <c r="B4" t="n">
         <v>859.0</v>
       </c>
+      <c r="C4" s="3" t="n">
+        <v>0.8598598598598599</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -173,6 +189,9 @@
       <c r="B5" t="n">
         <v>999.0</v>
       </c>
+      <c r="C5" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -183,6 +202,9 @@
       <c r="B6" t="n">
         <v>967.0</v>
       </c>
+      <c r="C6" s="3" t="n">
+        <v>0.9679679679679679</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
@@ -193,6 +215,9 @@
       <c r="B7" t="n">
         <v>7.0</v>
       </c>
+      <c r="C7" s="3" t="n">
+        <v>0.007238883143743537</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -203,6 +228,9 @@
       <c r="B8" t="n">
         <v>992.0</v>
       </c>
+      <c r="C8" s="3" t="n">
+        <v>0.992992992992993</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -213,9 +241,12 @@
       <c r="B9" t="n">
         <v>32.0</v>
       </c>
+      <c r="C9" s="3" t="n">
+        <v>0.03225806451612903</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9"/>
+  <autoFilter ref="A1:C9"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -230,6 +261,7 @@
   <cols>
     <col min="1" max="1" width="35.66015625" customWidth="true"/>
     <col min="2" max="2" width="10.32421875" customWidth="true"/>
+    <col min="3" max="3" width="12.4609375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -243,6 +275,11 @@
           <t>Value</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Relative</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -253,6 +290,9 @@
       <c r="B2" t="n">
         <v>140.0</v>
       </c>
+      <c r="C2" s="3" t="n">
+        <v>0.14477766287487073</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -263,6 +303,9 @@
       <c r="B3" t="n">
         <v>960.0</v>
       </c>
+      <c r="C3" s="3" t="n">
+        <v>0.9927611168562565</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -273,6 +316,9 @@
       <c r="B4" t="n">
         <v>827.0</v>
       </c>
+      <c r="C4" s="3" t="n">
+        <v>0.8552223371251293</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -283,6 +329,9 @@
       <c r="B5" t="n">
         <v>967.0</v>
       </c>
+      <c r="C5" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -293,6 +342,9 @@
       <c r="B6" t="n">
         <v>967.0</v>
       </c>
+      <c r="C6" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
@@ -303,6 +355,9 @@
       <c r="B7" t="n">
         <v>7.0</v>
       </c>
+      <c r="C7" s="3" t="n">
+        <v>0.007238883143743537</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -313,6 +368,9 @@
       <c r="B8" t="n">
         <v>960.0</v>
       </c>
+      <c r="C8" s="3" t="n">
+        <v>0.9927611168562565</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -323,9 +381,12 @@
       <c r="B9" t="n">
         <v>0.0</v>
       </c>
+      <c r="C9" s="3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9"/>
+  <autoFilter ref="A1:C9"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -340,6 +401,7 @@
   <cols>
     <col min="1" max="1" width="35.66015625" customWidth="true"/>
     <col min="2" max="2" width="10.32421875" customWidth="true"/>
+    <col min="3" max="3" width="12.4609375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -353,6 +415,11 @@
           <t>Value</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Relative</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -363,6 +430,9 @@
       <c r="B2" t="n">
         <v>140.0</v>
       </c>
+      <c r="C2" s="3" t="n">
+        <v>0.14112903225806453</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -373,6 +443,9 @@
       <c r="B3" t="n">
         <v>960.0</v>
       </c>
+      <c r="C3" s="3" t="n">
+        <v>0.967741935483871</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -383,6 +456,9 @@
       <c r="B4" t="n">
         <v>852.0</v>
       </c>
+      <c r="C4" s="3" t="n">
+        <v>0.8588709677419355</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -393,6 +469,9 @@
       <c r="B5" t="n">
         <v>992.0</v>
       </c>
+      <c r="C5" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -403,6 +482,9 @@
       <c r="B6" t="n">
         <v>960.0</v>
       </c>
+      <c r="C6" s="3" t="n">
+        <v>0.967741935483871</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
@@ -413,6 +495,9 @@
       <c r="B7" t="n">
         <v>0.0</v>
       </c>
+      <c r="C7" s="3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -423,6 +508,9 @@
       <c r="B8" t="n">
         <v>992.0</v>
       </c>
+      <c r="C8" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -433,9 +521,12 @@
       <c r="B9" t="n">
         <v>32.0</v>
       </c>
+      <c r="C9" s="3" t="n">
+        <v>0.03225806451612903</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9"/>
+  <autoFilter ref="A1:C9"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -450,6 +541,7 @@
   <cols>
     <col min="1" max="1" width="35.66015625" customWidth="true"/>
     <col min="2" max="2" width="10.32421875" customWidth="true"/>
+    <col min="3" max="3" width="12.4609375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -463,6 +555,11 @@
           <t>Value</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Relative</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -471,7 +568,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>960.0</v>
+        <v>140.0</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="3">
@@ -483,6 +583,9 @@
       <c r="B3" t="n">
         <v>960.0</v>
       </c>
+      <c r="C3" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -491,7 +594,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0</v>
+        <v>820.0</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0.8541666666666666</v>
       </c>
     </row>
     <row r="5">
@@ -503,6 +609,9 @@
       <c r="B5" t="n">
         <v>960.0</v>
       </c>
+      <c r="C5" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -513,6 +622,9 @@
       <c r="B6" t="n">
         <v>960.0</v>
       </c>
+      <c r="C6" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
@@ -523,6 +635,9 @@
       <c r="B7" t="n">
         <v>0.0</v>
       </c>
+      <c r="C7" s="3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -533,6 +648,9 @@
       <c r="B8" t="n">
         <v>960.0</v>
       </c>
+      <c r="C8" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -543,9 +661,12 @@
       <c r="B9" t="n">
         <v>0.0</v>
       </c>
+      <c r="C9" s="3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9"/>
+  <autoFilter ref="A1:C9"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -560,6 +681,7 @@
   <cols>
     <col min="1" max="1" width="35.66015625" customWidth="true"/>
     <col min="2" max="2" width="10.32421875" customWidth="true"/>
+    <col min="3" max="3" width="12.4609375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -573,6 +695,11 @@
           <t>Value</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Relative</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -583,6 +710,9 @@
       <c r="B2" t="n">
         <v>0.0</v>
       </c>
+      <c r="C2" s="3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -593,6 +723,9 @@
       <c r="B3" t="n">
         <v>0.0</v>
       </c>
+      <c r="C3" s="3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -603,6 +736,9 @@
       <c r="B4" t="n">
         <v>39.0</v>
       </c>
+      <c r="C4" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -613,6 +749,9 @@
       <c r="B5" t="n">
         <v>39.0</v>
       </c>
+      <c r="C5" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -623,6 +762,9 @@
       <c r="B6" t="n">
         <v>7.0</v>
       </c>
+      <c r="C6" s="3" t="n">
+        <v>0.1794871794871795</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
@@ -633,6 +775,9 @@
       <c r="B7" t="n">
         <v>7.0</v>
       </c>
+      <c r="C7" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -643,6 +788,9 @@
       <c r="B8" t="n">
         <v>32.0</v>
       </c>
+      <c r="C8" s="3" t="n">
+        <v>0.8205128205128205</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -653,9 +801,12 @@
       <c r="B9" t="n">
         <v>32.0</v>
       </c>
+      <c r="C9" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9"/>
+  <autoFilter ref="A1:C9"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -670,6 +821,7 @@
   <cols>
     <col min="1" max="1" width="35.66015625" customWidth="true"/>
     <col min="2" max="2" width="10.32421875" customWidth="true"/>
+    <col min="3" max="3" width="12.4609375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -683,6 +835,11 @@
           <t>Value</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Relative</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -693,6 +850,9 @@
       <c r="B2" t="n">
         <v>0.0</v>
       </c>
+      <c r="C2" s="3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -703,6 +863,9 @@
       <c r="B3" t="n">
         <v>0.0</v>
       </c>
+      <c r="C3" s="3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -713,6 +876,9 @@
       <c r="B4" t="n">
         <v>7.0</v>
       </c>
+      <c r="C4" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -723,6 +889,9 @@
       <c r="B5" t="n">
         <v>7.0</v>
       </c>
+      <c r="C5" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -733,6 +902,9 @@
       <c r="B6" t="n">
         <v>7.0</v>
       </c>
+      <c r="C6" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
@@ -743,6 +915,9 @@
       <c r="B7" t="n">
         <v>7.0</v>
       </c>
+      <c r="C7" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -753,6 +928,9 @@
       <c r="B8" t="n">
         <v>0.0</v>
       </c>
+      <c r="C8" s="3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -763,9 +941,14 @@
       <c r="B9" t="n">
         <v>0.0</v>
       </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>&lt;NaN&gt;</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9"/>
+  <autoFilter ref="A1:C9"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -780,6 +963,7 @@
   <cols>
     <col min="1" max="1" width="35.66015625" customWidth="true"/>
     <col min="2" max="2" width="10.32421875" customWidth="true"/>
+    <col min="3" max="3" width="12.4609375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -793,6 +977,11 @@
           <t>Value</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Relative</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -803,6 +992,9 @@
       <c r="B2" t="n">
         <v>0.0</v>
       </c>
+      <c r="C2" s="3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -813,6 +1005,9 @@
       <c r="B3" t="n">
         <v>0.0</v>
       </c>
+      <c r="C3" s="3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -823,6 +1018,9 @@
       <c r="B4" t="n">
         <v>32.0</v>
       </c>
+      <c r="C4" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -833,6 +1031,9 @@
       <c r="B5" t="n">
         <v>32.0</v>
       </c>
+      <c r="C5" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -843,6 +1044,9 @@
       <c r="B6" t="n">
         <v>0.0</v>
       </c>
+      <c r="C6" s="3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
@@ -853,6 +1057,11 @@
       <c r="B7" t="n">
         <v>0.0</v>
       </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>&lt;NaN&gt;</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -863,6 +1072,9 @@
       <c r="B8" t="n">
         <v>32.0</v>
       </c>
+      <c r="C8" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -873,9 +1085,12 @@
       <c r="B9" t="n">
         <v>32.0</v>
       </c>
+      <c r="C9" s="3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9"/>
+  <autoFilter ref="A1:C9"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* Added the tests form column limits in the result. * Changed format of the result status dump. * Other minor fixes related to added tests.
</commit_message>
<xml_diff>
--- a/tests/data/desired/summaryreport.xlsx
+++ b/tests/data/desired/summaryreport.xlsx
@@ -148,10 +148,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>140.0</v>
+        <v>604.0</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>0.14014014014014015</v>
+        <v>0.6046046046046046</v>
       </c>
     </row>
     <row r="3">
@@ -174,10 +174,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>859.0</v>
+        <v>395.0</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0.8598598598598599</v>
+        <v>0.3953953953953954</v>
       </c>
     </row>
     <row r="5">
@@ -288,10 +288,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>140.0</v>
+        <v>604.0</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>0.14477766287487073</v>
+        <v>0.6246122026887281</v>
       </c>
     </row>
     <row r="3">
@@ -314,10 +314,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>827.0</v>
+        <v>363.0</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0.8552223371251293</v>
+        <v>0.375387797311272</v>
       </c>
     </row>
     <row r="5">
@@ -428,10 +428,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>140.0</v>
+        <v>604.0</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>0.14112903225806453</v>
+        <v>0.6088709677419355</v>
       </c>
     </row>
     <row r="3">
@@ -454,10 +454,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>852.0</v>
+        <v>388.0</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0.8588709677419355</v>
+        <v>0.3911290322580645</v>
       </c>
     </row>
     <row r="5">
@@ -568,10 +568,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>140.0</v>
+        <v>604.0</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>0.14583333333333334</v>
+        <v>0.6291666666666667</v>
       </c>
     </row>
     <row r="3">
@@ -594,10 +594,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>820.0</v>
+        <v>356.0</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0.8541666666666666</v>
+        <v>0.37083333333333335</v>
       </c>
     </row>
     <row r="5">

</xml_diff>